<commit_message>
Worked on more Statistics
</commit_message>
<xml_diff>
--- a/08_Statistics/Calculator.xlsx
+++ b/08_Statistics/Calculator.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Population Paramters</t>
   </si>
@@ -48,6 +48,48 @@
   </si>
   <si>
     <t>Z Score</t>
+  </si>
+  <si>
+    <t>t Statistics</t>
+  </si>
+  <si>
+    <t>Population Details</t>
+  </si>
+  <si>
+    <t>Sample Population Details</t>
+  </si>
+  <si>
+    <t>t Score</t>
+  </si>
+  <si>
+    <t>Cohen's d</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>n1</t>
+  </si>
+  <si>
+    <t>n2</t>
+  </si>
+  <si>
+    <t>SS1</t>
+  </si>
+  <si>
+    <t>SS2</t>
+  </si>
+  <si>
+    <t>Sp^2</t>
+  </si>
+  <si>
+    <t>t stats</t>
+  </si>
+  <si>
+    <t>df</t>
   </si>
 </sst>
 </file>
@@ -83,12 +125,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -384,16 +429,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -441,10 +486,149 @@
         <v>16.964950524944058</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="D13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1830</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <f>(E14-B14)/(E15/SQRT(E16))</f>
+        <v>-3.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <f>(E14-B14)/E15</f>
+        <v>-0.65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24">
+        <v>207</v>
+      </c>
+      <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>31.6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25">
+        <v>220</v>
+      </c>
+      <c r="G25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27">
+        <f>(H24+H25) / (E27)</f>
+        <v>1.8894117647058823</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27">
+        <f>E24+E25-2</f>
+        <v>425</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <f>SQRT( ( (B27^2) / E24) + ( (B27^2) / E25) )</f>
+        <v>0.18295489751716662</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <f>(B24-B25)/B28</f>
+        <v>22.956477563580449</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>